<commit_message>
sprint 12(organization address incactive and active)
</commit_message>
<xml_diff>
--- a/media/reports/All_Input_Yearly.xlsx
+++ b/media/reports/All_Input_Yearly.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reports" sheetId="1" state="visible" r:id="rId1"/>
@@ -68,17 +68,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,7 +455,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>akhil</t>
         </is>
       </c>
     </row>
@@ -467,7 +467,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>org name</t>
+          <t>fkjds</t>
         </is>
       </c>
     </row>
@@ -495,7 +495,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2020-07-30</t>
+          <t>2020-08-11</t>
         </is>
       </c>
     </row>
@@ -541,12 +541,12 @@
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>2020-07-29</t>
+          <t>2020-08-08</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>register</t>
+          <t>DJFLDSK</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
@@ -560,18 +560,18 @@
         </is>
       </c>
       <c r="E10" s="2" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>2020-07-30</t>
+          <t>2020-08-08</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>register</t>
+          <t>DKJFHKDJ</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr">
@@ -585,21 +585,71 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
-      <c r="D12" s="1" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>2020-08-10</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>DJFLDSK</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>IN-0003</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>INVOICE</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>2020-08-11</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>44444444444</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>IN-0004</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>INVOICE</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>4012.8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="D14" s="1" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="E12" s="1">
-        <f> SUM(E10:E11)</f>
+      <c r="E14" s="1">
+        <f> SUM(E10:E13)</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>